<commit_message>
Modified, excel sizes & evaluateBracketsInProduct
</commit_message>
<xml_diff>
--- a/public/excel/FormularioDePedidos.xlsx
+++ b/public/excel/FormularioDePedidos.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28528"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05B0677B-6D18-4E1F-A051-4D61F2099F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F06019DB-BE7E-4070-A078-DCC1B919955D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,15 +73,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -89,19 +84,8 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="14"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -193,29 +177,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,10 +326,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="D6" sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -356,63 +339,76 @@
     <col min="3" max="3" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="18">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:4" ht="18">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="20.25">
-      <c r="A3" s="1" t="s">
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" ht="18">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="23.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" ht="18">
-      <c r="A7" s="7" t="s">
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" ht="18">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" ht="18">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" ht="18">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="35" spans="2:2" ht="18">
-      <c r="B35" s="7"/>
+      <c r="B35" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>